<commit_message>
Calibration corrections for BHRbEF, BHNVFEAL, BNVFE, and BPoEFUbVT
</commit_message>
<xml_diff>
--- a/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
+++ b/InputData/trans/BHNVFEAL/BAU Historical New Veh Fuel Economy After Lifetime.xlsx
@@ -4748,178 +4748,178 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="70"/>
                 <c:pt idx="12" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="13" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="14" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="15" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="16" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="17" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="18" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="19" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="20" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="21" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="22" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="23" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="24" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="25" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="26" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="27" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="28" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="29" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="30" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="31" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="32" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="33" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="34" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="35" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="36" formatCode="0.00E+00">
-                  <c:v>6.1890223381182868E-4</c:v>
+                  <c:v>6.0313010134796052E-4</c:v>
                 </c:pt>
                 <c:pt idx="37" formatCode="0.00E+00">
-                  <c:v>6.2694796285138238E-4</c:v>
+                  <c:v>6.072320057266767E-4</c:v>
                 </c:pt>
                 <c:pt idx="38" formatCode="0.00E+00">
-                  <c:v>6.3509828636845028E-4</c:v>
+                  <c:v>6.1181381950663899E-4</c:v>
                 </c:pt>
                 <c:pt idx="39" formatCode="0.00E+00">
-                  <c:v>6.4335456409124003E-4</c:v>
+                  <c:v>6.2383232505965926E-4</c:v>
                 </c:pt>
                 <c:pt idx="40" formatCode="0.00E+00">
-                  <c:v>6.517181734244261E-4</c:v>
+                  <c:v>6.3603424104160589E-4</c:v>
                 </c:pt>
                 <c:pt idx="41" formatCode="0.00E+00">
-                  <c:v>6.6019050967894353E-4</c:v>
+                  <c:v>6.4894526301838707E-4</c:v>
                 </c:pt>
                 <c:pt idx="42" formatCode="0.00E+00">
-                  <c:v>6.6877298630476972E-4</c:v>
+                  <c:v>6.6244996523030493E-4</c:v>
                 </c:pt>
                 <c:pt idx="43" formatCode="0.00E+00">
-                  <c:v>6.7746703512673167E-4</c:v>
+                  <c:v>6.7656034063432705E-4</c:v>
                 </c:pt>
                 <c:pt idx="44" formatCode="0.00E+00">
-                  <c:v>6.8627410658337912E-4</c:v>
+                  <c:v>6.9128948265566868E-4</c:v>
                 </c:pt>
                 <c:pt idx="45" formatCode="0.00E+00">
-                  <c:v>6.9519566996896303E-4</c:v>
+                  <c:v>7.0665156633416737E-4</c:v>
                 </c:pt>
                 <c:pt idx="46" formatCode="0.00E+00">
-                  <c:v>7.0423321367855951E-4</c:v>
+                  <c:v>7.2266183528083645E-4</c:v>
                 </c:pt>
                 <c:pt idx="47" formatCode="0.00E+00">
-                  <c:v>7.1338824545638072E-4</c:v>
+                  <c:v>7.3933659385631736E-4</c:v>
                 </c:pt>
                 <c:pt idx="48" formatCode="0.00E+00">
-                  <c:v>7.2266229264731361E-4</c:v>
+                  <c:v>7.5669320407387175E-4</c:v>
                 </c:pt>
                 <c:pt idx="49" formatCode="0.00E+00">
-                  <c:v>7.3205690245172861E-4</c:v>
+                  <c:v>7.7475008680641833E-4</c:v>
                 </c:pt>
                 <c:pt idx="50" formatCode="0.00E+00">
-                  <c:v>7.4157364218360104E-4</c:v>
+                  <c:v>7.9863335786483529E-4</c:v>
                 </c:pt>
                 <c:pt idx="51" formatCode="0.00E+00">
-                  <c:v>7.5121409953198773E-4</c:v>
+                  <c:v>8.237234232157186E-4</c:v>
                 </c:pt>
                 <c:pt idx="52" formatCode="0.00E+00">
-                  <c:v>7.6097988282590348E-4</c:v>
+                  <c:v>8.5007053965037362E-4</c:v>
                 </c:pt>
                 <c:pt idx="53" formatCode="0.00E+00">
-                  <c:v>7.7087262130264012E-4</c:v>
+                  <c:v>8.7772798200527345E-4</c:v>
                 </c:pt>
                 <c:pt idx="54" formatCode="0.00E+00">
-                  <c:v>7.8089396537957441E-4</c:v>
+                  <c:v>9.0675215827171586E-4</c:v>
                 </c:pt>
                 <c:pt idx="55" formatCode="0.00E+00">
-                  <c:v>7.9104558692950878E-4</c:v>
+                  <c:v>9.3720273489263269E-4</c:v>
                 </c:pt>
                 <c:pt idx="56" formatCode="0.00E+00">
-                  <c:v>8.0132917955959228E-4</c:v>
+                  <c:v>9.6914277233677872E-4</c:v>
                 </c:pt>
                 <c:pt idx="57" formatCode="0.00E+00">
-                  <c:v>8.1174645889386693E-4</c:v>
+                  <c:v>1.0026388711041254E-3</c:v>
                 </c:pt>
                 <c:pt idx="58" formatCode="0.00E+00">
-                  <c:v>8.2229916285948715E-4</c:v>
+                  <c:v>1.0377613283751872E-3</c:v>
                 </c:pt>
                 <c:pt idx="59" formatCode="0.00E+00">
-                  <c:v>8.3298905197666041E-4</c:v>
+                  <c:v>1.074584305572199E-3</c:v>
                 </c:pt>
                 <c:pt idx="60" formatCode="0.00E+00">
-                  <c:v>8.4381790965235687E-4</c:v>
+                  <c:v>1.1137282028841316E-3</c:v>
                 </c:pt>
                 <c:pt idx="61" formatCode="0.00E+00">
-                  <c:v>8.5478754247783747E-4</c:v>
+                  <c:v>1.1547726751853448E-3</c:v>
                 </c:pt>
                 <c:pt idx="62" formatCode="0.00E+00">
-                  <c:v>8.6589978053004928E-4</c:v>
+                  <c:v>1.197807450156568E-3</c:v>
                 </c:pt>
                 <c:pt idx="63" formatCode="0.00E+00">
-                  <c:v>8.7715647767693981E-4</c:v>
+                  <c:v>1.2429270853403414E-3</c:v>
                 </c:pt>
                 <c:pt idx="64" formatCode="0.00E+00">
-                  <c:v>8.8855951188673995E-4</c:v>
+                  <c:v>1.2902312080237291E-3</c:v>
                 </c:pt>
                 <c:pt idx="65" formatCode="0.00E+00">
-                  <c:v>9.0011078554126753E-4</c:v>
+                  <c:v>1.3398247693971758E-3</c:v>
                 </c:pt>
                 <c:pt idx="66" formatCode="0.00E+00">
-                  <c:v>9.1181222575330387E-4</c:v>
+                  <c:v>1.3918183136469805E-3</c:v>
                 </c:pt>
                 <c:pt idx="67" formatCode="0.00E+00">
-                  <c:v>9.2366578468809678E-4</c:v>
+                  <c:v>1.4463282626894839E-3</c:v>
                 </c:pt>
                 <c:pt idx="68" formatCode="0.00E+00">
-                  <c:v>9.356734398890419E-4</c:v>
+                  <c:v>1.5034772173068065E-3</c:v>
                 </c:pt>
                 <c:pt idx="69" formatCode="0.00E+00">
-                  <c:v>9.4783719460759933E-4</c:v>
+                  <c:v>1.5633942754972108E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8231,139 +8231,139 @@
       </c>
       <c r="B2" s="4">
         <f>B$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="C2" s="4">
         <f>C$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="D2" s="4">
         <f>D$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="E2" s="4">
         <f>E$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="F2" s="4">
         <f>F$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="G2" s="4">
         <f>G$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="H2" s="4">
         <f>H$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="I2" s="4">
         <f>I$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="J2" s="4">
         <f>J$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="K2" s="4">
         <f>K$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="L2" s="4">
         <f>L$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="M2" s="4">
         <f>M$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="N2" s="4">
         <f>N$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="O2" s="4">
         <f>O$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="P2" s="4">
         <f>P$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="Q2" s="4">
         <f>Q$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="R2" s="4">
         <f>R$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="S2" s="4">
         <f>S$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="T2" s="4">
         <f>T$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="U2" s="4">
         <f>U$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="V2" s="4">
         <f>V$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="W2" s="4">
         <f>W$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="X2" s="4">
         <f>X$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="Y2" s="4">
         <f>Y$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="Z2" s="4">
         <f>Z$5/(1-'Other Values'!$B$3)</f>
-        <v>1.9888266332560279E-3</v>
+        <v>1.9381432855579805E-3</v>
       </c>
       <c r="AA2" s="4">
         <f>AA$5/(1-'Other Values'!$B$3)</f>
-        <v>2.014681379488356E-3</v>
+        <v>1.9513246512564289E-3</v>
       </c>
       <c r="AB2" s="4">
         <f>AB$5/(1-'Other Values'!$B$3)</f>
-        <v>2.0408722374217043E-3</v>
+        <v>1.9660481936454826E-3</v>
       </c>
       <c r="AC2" s="4">
         <f>AC$5/(1-'Other Values'!$B$3)</f>
-        <v>2.067403576508186E-3</v>
+        <v>2.004669356455907E-3</v>
       </c>
       <c r="AD2" s="4">
         <f>AD$5/(1-'Other Values'!$B$3)</f>
-        <v>2.0942798230027923E-3</v>
+        <v>2.043879904028476E-3</v>
       </c>
       <c r="AE2" s="4">
         <f>AE$5/(1-'Other Values'!$B$3)</f>
-        <v>2.1215054607018283E-3</v>
+        <v>2.0853691457328183E-3</v>
       </c>
       <c r="AF2" s="4">
         <f>AF$5/(1-'Other Values'!$B$3)</f>
-        <v>2.1490850316909517E-3</v>
+        <v>2.1287661638172933E-3</v>
       </c>
       <c r="AG2" s="4">
         <f>AG$5/(1-'Other Values'!$B$3)</f>
-        <v>2.1770231371029342E-3</v>
+        <v>2.1741094973449799E-3</v>
       </c>
       <c r="AH2" s="4">
         <f>AH$5/(1-'Other Values'!$B$3)</f>
-        <v>2.2053244378852721E-3</v>
+        <v>2.2214412217057633E-3</v>
       </c>
       <c r="AI2" s="4">
         <f>AI$5/(1-'Other Values'!$B$3)</f>
-        <v>2.2339936555777805E-3</v>
+        <v>2.2708068880306891E-3</v>
       </c>
     </row>
     <row r="3" spans="1:35">
@@ -8586,139 +8586,139 @@
       </c>
       <c r="B5" s="4">
         <f>Extrapolations!O6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="C5" s="4">
         <f>Extrapolations!P6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="D5" s="4">
         <f>Extrapolations!Q6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="E5" s="4">
         <f>Extrapolations!R6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="F5" s="4">
         <f>Extrapolations!S6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="G5" s="4">
         <f>Extrapolations!T6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="H5" s="4">
         <f>Extrapolations!U6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="I5" s="4">
         <f>Extrapolations!V6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="J5" s="4">
         <f>Extrapolations!W6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="K5" s="4">
         <f>Extrapolations!X6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="L5" s="4">
         <f>Extrapolations!Y6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="M5" s="4">
         <f>Extrapolations!Z6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="N5" s="4">
         <f>Extrapolations!AA6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="O5" s="4">
         <f>Extrapolations!AB6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="P5" s="4">
         <f>Extrapolations!AC6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="Q5" s="4">
         <f>Extrapolations!AD6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="R5" s="4">
         <f>Extrapolations!AE6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="S5" s="4">
         <f>Extrapolations!AF6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="T5" s="4">
         <f>Extrapolations!AG6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="U5" s="4">
         <f>Extrapolations!AH6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="V5" s="4">
         <f>Extrapolations!AI6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="W5" s="4">
         <f>Extrapolations!AJ6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="X5" s="4">
         <f>Extrapolations!AK6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="Y5" s="4">
         <f>Extrapolations!AL6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="Z5" s="4">
         <f>Extrapolations!AM6</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AA5" s="4">
         <f>Extrapolations!AN6</f>
-        <v>6.2694796285138238E-4</v>
+        <v>6.072320057266767E-4</v>
       </c>
       <c r="AB5" s="4">
         <f>Extrapolations!AO6</f>
-        <v>6.3509828636845028E-4</v>
+        <v>6.1181381950663899E-4</v>
       </c>
       <c r="AC5" s="4">
         <f>Extrapolations!AP6</f>
-        <v>6.4335456409124003E-4</v>
+        <v>6.2383232505965926E-4</v>
       </c>
       <c r="AD5" s="4">
         <f>Extrapolations!AQ6</f>
-        <v>6.517181734244261E-4</v>
+        <v>6.3603424104160589E-4</v>
       </c>
       <c r="AE5" s="4">
         <f>Extrapolations!AR6</f>
-        <v>6.6019050967894353E-4</v>
+        <v>6.4894526301838707E-4</v>
       </c>
       <c r="AF5" s="4">
         <f>Extrapolations!AS6</f>
-        <v>6.6877298630476972E-4</v>
+        <v>6.6244996523030493E-4</v>
       </c>
       <c r="AG5" s="4">
         <f>Extrapolations!AT6</f>
-        <v>6.7746703512673167E-4</v>
+        <v>6.7656034063432705E-4</v>
       </c>
       <c r="AH5" s="4">
         <f>Extrapolations!AU6</f>
-        <v>6.8627410658337912E-4</v>
+        <v>6.9128948265566868E-4</v>
       </c>
       <c r="AI5" s="4">
         <f>Extrapolations!AV6</f>
-        <v>6.9519566996896303E-4</v>
+        <v>7.0665156633416737E-4</v>
       </c>
     </row>
     <row r="6" spans="1:35">
@@ -8941,139 +8941,139 @@
       </c>
       <c r="B8" s="4">
         <f>B$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="C8" s="4">
         <f>C$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="D8" s="4">
         <f>D$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="E8" s="4">
         <f>E$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="F8" s="4">
         <f>F$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="G8" s="4">
         <f>G$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="H8" s="4">
         <f>H$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="I8" s="4">
         <f>I$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="J8" s="4">
         <f>J$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="K8" s="4">
         <f>K$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="L8" s="4">
         <f>L$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="M8" s="4">
         <f>M$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="N8" s="4">
         <f>N$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="O8" s="4">
         <f>O$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="P8" s="4">
         <f>P$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="Q8" s="4">
         <f>Q$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="R8" s="4">
         <f>R$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="S8" s="4">
         <f>S$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="T8" s="4">
         <f>T$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="U8" s="4">
         <f>U$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="V8" s="4">
         <f>V$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="W8" s="4">
         <f>W$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="X8" s="4">
         <f>X$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="Y8" s="4">
         <f>Y$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="Z8" s="4">
         <f>Z$5*Calculations!$B$27</f>
-        <v>1.5472555845295716E-3</v>
+        <v>1.5078252533699014E-3</v>
       </c>
       <c r="AA8" s="4">
         <f>AA$5*Calculations!$B$27</f>
-        <v>1.567369907128456E-3</v>
+        <v>1.5180800143166917E-3</v>
       </c>
       <c r="AB8" s="4">
         <f>AB$5*Calculations!$B$27</f>
-        <v>1.5877457159211258E-3</v>
+        <v>1.5295345487665974E-3</v>
       </c>
       <c r="AC8" s="4">
         <f>AC$5*Calculations!$B$27</f>
-        <v>1.6083864102281E-3</v>
+        <v>1.5595808126491481E-3</v>
       </c>
       <c r="AD8" s="4">
         <f>AD$5*Calculations!$B$27</f>
-        <v>1.6292954335610653E-3</v>
+        <v>1.5900856026040146E-3</v>
       </c>
       <c r="AE8" s="4">
         <f>AE$5*Calculations!$B$27</f>
-        <v>1.6504762741973589E-3</v>
+        <v>1.6223631575459677E-3</v>
       </c>
       <c r="AF8" s="4">
         <f>AF$5*Calculations!$B$27</f>
-        <v>1.6719324657619244E-3</v>
+        <v>1.6561249130757623E-3</v>
       </c>
       <c r="AG8" s="4">
         <f>AG$5*Calculations!$B$27</f>
-        <v>1.6936675878168291E-3</v>
+        <v>1.6914008515858175E-3</v>
       </c>
       <c r="AH8" s="4">
         <f>AH$5*Calculations!$B$27</f>
-        <v>1.7156852664584478E-3</v>
+        <v>1.7282237066391717E-3</v>
       </c>
       <c r="AI8" s="4">
         <f>AI$5*Calculations!$B$27</f>
-        <v>1.7379891749224076E-3</v>
+        <v>1.7666289158354185E-3</v>
       </c>
     </row>
   </sheetData>
@@ -15834,8 +15834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:AM13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:AM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -16521,106 +16521,106 @@
         <v>6.1095975697120306E-4</v>
       </c>
       <c r="F12" s="42">
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="G12" s="4">
-        <v>6.2694796285138238E-4</v>
+        <v>6.072320057266767E-4</v>
       </c>
       <c r="H12" s="4">
-        <v>6.3509828636845028E-4</v>
+        <v>6.1181381950663899E-4</v>
       </c>
       <c r="I12" s="4">
-        <v>6.4335456409124003E-4</v>
+        <v>6.2383232505965926E-4</v>
       </c>
       <c r="J12" s="4">
-        <v>6.517181734244261E-4</v>
+        <v>6.3603424104160589E-4</v>
       </c>
       <c r="K12" s="4">
-        <v>6.6019050967894353E-4</v>
+        <v>6.4894526301838707E-4</v>
       </c>
       <c r="L12" s="4">
-        <v>6.6877298630476972E-4</v>
+        <v>6.6244996523030493E-4</v>
       </c>
       <c r="M12" s="4">
-        <v>6.7746703512673167E-4</v>
+        <v>6.7656034063432705E-4</v>
       </c>
       <c r="N12" s="4">
-        <v>6.8627410658337912E-4</v>
+        <v>6.9128948265566868E-4</v>
       </c>
       <c r="O12" s="4">
-        <v>6.9519566996896303E-4</v>
+        <v>7.0665156633416737E-4</v>
       </c>
       <c r="P12" s="4">
-        <v>7.0423321367855951E-4</v>
+        <v>7.2266183528083645E-4</v>
       </c>
       <c r="Q12" s="4">
-        <v>7.1338824545638072E-4</v>
+        <v>7.3933659385631736E-4</v>
       </c>
       <c r="R12" s="4">
-        <v>7.2266229264731361E-4</v>
+        <v>7.5669320407387175E-4</v>
       </c>
       <c r="S12" s="4">
-        <v>7.3205690245172861E-4</v>
+        <v>7.7475008680641833E-4</v>
       </c>
       <c r="T12" s="4">
-        <v>7.4157364218360104E-4</v>
+        <v>7.9863335786483529E-4</v>
       </c>
       <c r="U12" s="4">
-        <v>7.5121409953198773E-4</v>
+        <v>8.237234232157186E-4</v>
       </c>
       <c r="V12" s="4">
-        <v>7.6097988282590348E-4</v>
+        <v>8.5007053965037362E-4</v>
       </c>
       <c r="W12" s="4">
-        <v>7.7087262130264012E-4</v>
+        <v>8.7772798200527345E-4</v>
       </c>
       <c r="X12" s="4">
-        <v>7.8089396537957441E-4</v>
+        <v>9.0675215827171586E-4</v>
       </c>
       <c r="Y12" s="4">
-        <v>7.9104558692950878E-4</v>
+        <v>9.3720273489263269E-4</v>
       </c>
       <c r="Z12" s="4">
-        <v>8.0132917955959228E-4</v>
+        <v>9.6914277233677872E-4</v>
       </c>
       <c r="AA12" s="4">
-        <v>8.1174645889386693E-4</v>
+        <v>1.0026388711041254E-3</v>
       </c>
       <c r="AB12" s="4">
-        <v>8.2229916285948715E-4</v>
+        <v>1.0377613283751872E-3</v>
       </c>
       <c r="AC12" s="4">
-        <v>8.3298905197666041E-4</v>
+        <v>1.074584305572199E-3</v>
       </c>
       <c r="AD12" s="4">
-        <v>8.4381790965235687E-4</v>
+        <v>1.1137282028841316E-3</v>
       </c>
       <c r="AE12" s="4">
-        <v>8.5478754247783747E-4</v>
+        <v>1.1547726751853448E-3</v>
       </c>
       <c r="AF12" s="4">
-        <v>8.6589978053004928E-4</v>
+        <v>1.197807450156568E-3</v>
       </c>
       <c r="AG12" s="4">
-        <v>8.7715647767693981E-4</v>
+        <v>1.2429270853403414E-3</v>
       </c>
       <c r="AH12" s="4">
-        <v>8.8855951188673995E-4</v>
+        <v>1.2902312080237291E-3</v>
       </c>
       <c r="AI12" s="4">
-        <v>9.0011078554126753E-4</v>
+        <v>1.3398247693971758E-3</v>
       </c>
       <c r="AJ12" s="4">
-        <v>9.1181222575330387E-4</v>
+        <v>1.3918183136469805E-3</v>
       </c>
       <c r="AK12" s="4">
-        <v>9.2366578468809678E-4</v>
+        <v>1.4463282626894839E-3</v>
       </c>
       <c r="AL12" s="4">
-        <v>9.356734398890419E-4</v>
+        <v>1.5034772173068065E-3</v>
       </c>
       <c r="AM12" s="4">
-        <v>9.4783719460759933E-4</v>
+        <v>1.5633942754972108E-3</v>
       </c>
       <c r="AN12" s="4"/>
     </row>
@@ -18860,235 +18860,235 @@
       <c r="N6" s="10"/>
       <c r="O6" s="14">
         <f t="shared" si="27"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="P6" s="14">
         <f t="shared" si="28"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="Q6" s="14">
         <f t="shared" si="29"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="R6" s="14">
         <f t="shared" si="30"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="S6" s="14">
         <f t="shared" si="31"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="T6" s="14">
         <f t="shared" si="32"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="U6" s="14">
         <f t="shared" si="33"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="V6" s="14">
         <f t="shared" si="34"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="W6" s="14">
         <f t="shared" si="35"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="X6" s="14">
         <f t="shared" si="36"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="Y6" s="14">
         <f t="shared" si="37"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="Z6" s="14">
         <f t="shared" si="38"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AA6" s="14">
         <f t="shared" si="39"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AB6" s="14">
         <f t="shared" si="40"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AC6" s="14">
         <f t="shared" si="41"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AD6" s="14">
         <f t="shared" si="42"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AE6" s="14">
         <f t="shared" si="43"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AF6" s="14">
         <f t="shared" si="44"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AG6" s="14">
         <f t="shared" si="45"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AH6" s="14">
         <f t="shared" si="46"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AI6" s="14">
         <f t="shared" si="47"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AJ6" s="14">
         <f t="shared" si="48"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AK6" s="14">
         <f t="shared" si="49"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AL6" s="14">
         <f t="shared" si="50"/>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AM6" s="40">
         <f>BNVFE!F12</f>
-        <v>6.1890223381182868E-4</v>
+        <v>6.0313010134796052E-4</v>
       </c>
       <c r="AN6" s="13">
         <f>BNVFE!G12</f>
-        <v>6.2694796285138238E-4</v>
+        <v>6.072320057266767E-4</v>
       </c>
       <c r="AO6" s="13">
         <f>BNVFE!H12</f>
-        <v>6.3509828636845028E-4</v>
+        <v>6.1181381950663899E-4</v>
       </c>
       <c r="AP6" s="13">
         <f>BNVFE!I12</f>
-        <v>6.4335456409124003E-4</v>
+        <v>6.2383232505965926E-4</v>
       </c>
       <c r="AQ6" s="13">
         <f>BNVFE!J12</f>
-        <v>6.517181734244261E-4</v>
+        <v>6.3603424104160589E-4</v>
       </c>
       <c r="AR6" s="13">
         <f>BNVFE!K12</f>
-        <v>6.6019050967894353E-4</v>
+        <v>6.4894526301838707E-4</v>
       </c>
       <c r="AS6" s="13">
         <f>BNVFE!L12</f>
-        <v>6.6877298630476972E-4</v>
+        <v>6.6244996523030493E-4</v>
       </c>
       <c r="AT6" s="13">
         <f>BNVFE!M12</f>
-        <v>6.7746703512673167E-4</v>
+        <v>6.7656034063432705E-4</v>
       </c>
       <c r="AU6" s="13">
         <f>BNVFE!N12</f>
-        <v>6.8627410658337912E-4</v>
+        <v>6.9128948265566868E-4</v>
       </c>
       <c r="AV6" s="13">
         <f>BNVFE!O12</f>
-        <v>6.9519566996896303E-4</v>
+        <v>7.0665156633416737E-4</v>
       </c>
       <c r="AW6" s="13">
         <f>BNVFE!P12</f>
-        <v>7.0423321367855951E-4</v>
+        <v>7.2266183528083645E-4</v>
       </c>
       <c r="AX6" s="13">
         <f>BNVFE!Q12</f>
-        <v>7.1338824545638072E-4</v>
+        <v>7.3933659385631736E-4</v>
       </c>
       <c r="AY6" s="13">
         <f>BNVFE!R12</f>
-        <v>7.2266229264731361E-4</v>
+        <v>7.5669320407387175E-4</v>
       </c>
       <c r="AZ6" s="13">
         <f>BNVFE!S12</f>
-        <v>7.3205690245172861E-4</v>
+        <v>7.7475008680641833E-4</v>
       </c>
       <c r="BA6" s="13">
         <f>BNVFE!T12</f>
-        <v>7.4157364218360104E-4</v>
+        <v>7.9863335786483529E-4</v>
       </c>
       <c r="BB6" s="13">
         <f>BNVFE!U12</f>
-        <v>7.5121409953198773E-4</v>
+        <v>8.237234232157186E-4</v>
       </c>
       <c r="BC6" s="13">
         <f>BNVFE!V12</f>
-        <v>7.6097988282590348E-4</v>
+        <v>8.5007053965037362E-4</v>
       </c>
       <c r="BD6" s="13">
         <f>BNVFE!W12</f>
-        <v>7.7087262130264012E-4</v>
+        <v>8.7772798200527345E-4</v>
       </c>
       <c r="BE6" s="13">
         <f>BNVFE!X12</f>
-        <v>7.8089396537957441E-4</v>
+        <v>9.0675215827171586E-4</v>
       </c>
       <c r="BF6" s="13">
         <f>BNVFE!Y12</f>
-        <v>7.9104558692950878E-4</v>
+        <v>9.3720273489263269E-4</v>
       </c>
       <c r="BG6" s="13">
         <f>BNVFE!Z12</f>
-        <v>8.0132917955959228E-4</v>
+        <v>9.6914277233677872E-4</v>
       </c>
       <c r="BH6" s="13">
         <f>BNVFE!AA12</f>
-        <v>8.1174645889386693E-4</v>
+        <v>1.0026388711041254E-3</v>
       </c>
       <c r="BI6" s="13">
         <f>BNVFE!AB12</f>
-        <v>8.2229916285948715E-4</v>
+        <v>1.0377613283751872E-3</v>
       </c>
       <c r="BJ6" s="13">
         <f>BNVFE!AC12</f>
-        <v>8.3298905197666041E-4</v>
+        <v>1.074584305572199E-3</v>
       </c>
       <c r="BK6" s="13">
         <f>BNVFE!AD12</f>
-        <v>8.4381790965235687E-4</v>
+        <v>1.1137282028841316E-3</v>
       </c>
       <c r="BL6" s="13">
         <f>BNVFE!AE12</f>
-        <v>8.5478754247783747E-4</v>
+        <v>1.1547726751853448E-3</v>
       </c>
       <c r="BM6" s="13">
         <f>BNVFE!AF12</f>
-        <v>8.6589978053004928E-4</v>
+        <v>1.197807450156568E-3</v>
       </c>
       <c r="BN6" s="13">
         <f>BNVFE!AG12</f>
-        <v>8.7715647767693981E-4</v>
+        <v>1.2429270853403414E-3</v>
       </c>
       <c r="BO6" s="13">
         <f>BNVFE!AH12</f>
-        <v>8.8855951188673995E-4</v>
+        <v>1.2902312080237291E-3</v>
       </c>
       <c r="BP6" s="13">
         <f>BNVFE!AI12</f>
-        <v>9.0011078554126753E-4</v>
+        <v>1.3398247693971758E-3</v>
       </c>
       <c r="BQ6" s="13">
         <f>BNVFE!AJ12</f>
-        <v>9.1181222575330387E-4</v>
+        <v>1.3918183136469805E-3</v>
       </c>
       <c r="BR6" s="13">
         <f>BNVFE!AK12</f>
-        <v>9.2366578468809678E-4</v>
+        <v>1.4463282626894839E-3</v>
       </c>
       <c r="BS6" s="13">
         <f>BNVFE!AL12</f>
-        <v>9.356734398890419E-4</v>
+        <v>1.5034772173068065E-3</v>
       </c>
       <c r="BT6" s="13">
         <f>BNVFE!AM12</f>
-        <v>9.4783719460759933E-4</v>
+        <v>1.5633942754972108E-3</v>
       </c>
     </row>
     <row r="7" spans="1:72" ht="15.75" customHeight="1">

</xml_diff>